<commit_message>
Se agrega la operacióm Módulo, y se resuleven problemas de identación que tenía el código, ya que no arojaba los resultados
</commit_message>
<xml_diff>
--- a/operaciones.xlsx
+++ b/operaciones.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,7 +510,43 @@
         <v>1728</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45735.92259595744</v>
+        <v>45735.92259596065</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>El Kevin</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2 Potencia 2</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45735.9545602662</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>El Kevin</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10 Módulo 3</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>45735.95928607793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SE agrega operacion Raíz a la calculadora
</commit_message>
<xml_diff>
--- a/operaciones.xlsx
+++ b/operaciones.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,7 +546,25 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>45735.95928607793</v>
+        <v>45735.95928607639</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Marvin</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>125 Raíz 2</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>11.18033988749895</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>45735.96277760838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega el README con instrucciones de udo
</commit_message>
<xml_diff>
--- a/operaciones.xlsx
+++ b/operaciones.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -564,7 +564,43 @@
         <v>11.18033988749895</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>45735.96277760838</v>
+        <v>45735.96277760417</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Marvin</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>15 Sumar 2</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>45735.96473391203</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Marvin</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>15 Raíz 2</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>3.872983346207417</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>45735.96477394013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>